<commit_message>
Borrar foto al eliminar el usuario
</commit_message>
<xml_diff>
--- a/upload/xls/register.xlsx
+++ b/upload/xls/register.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Consecutivo</t>
+          <t>Recibo</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>310000</t>
+          <t>310001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,12 +488,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>06/07/2024</t>
+          <t>08/07/2024 11:49:45</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>07/07/2024</t>
+          <t>08/07/2024 11:50:01</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -505,10 +505,262 @@
         <v>1500</v>
       </c>
       <c r="G2" t="n">
-        <v>49495</v>
+        <v>16</v>
       </c>
       <c r="H2" t="n">
-        <v>10000</v>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>310002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>08/07/2024 18:11:30</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>09/07/2024 12:12:09</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G3" t="n">
+        <v>64839</v>
+      </c>
+      <c r="H3" t="n">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>310003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BBB01</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>08/07/2024 18:11:38</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>09/07/2024 12:13:47</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G4" t="n">
+        <v>64929</v>
+      </c>
+      <c r="H4" t="n">
+        <v>14750</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>310004</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CCC01</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>08/07/2024 18:11:43</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>09/07/2024 12:14:26</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G5" t="n">
+        <v>64963</v>
+      </c>
+      <c r="H5" t="n">
+        <v>14750</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>310005</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>DDD01</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>08/07/2024 18:11:54</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>09/07/2024 15:13:41</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G6" t="n">
+        <v>75707</v>
+      </c>
+      <c r="H6" t="n">
+        <v>14750</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>310006</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>EEE01</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>08/07/2024 18:12:11</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>09/07/2024 15:14:11</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G7" t="n">
+        <v>75720</v>
+      </c>
+      <c r="H7" t="n">
+        <v>14750</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>310007</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>FFF01</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>08/07/2024 18:17:30</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>09/07/2024 15:15:15</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G8" t="n">
+        <v>75465</v>
+      </c>
+      <c r="H8" t="n">
+        <v>15500</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>310008</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>GGG01</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>08/07/2024 18:18:07</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>09/07/2024 15:15:26</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G9" t="n">
+        <v>75439</v>
+      </c>
+      <c r="H9" t="n">
+        <v>15500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregó el ancho del papel para recibos y factura en configuración
</commit_message>
<xml_diff>
--- a/upload/xls/register.xlsx
+++ b/upload/xls/register.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>310001</t>
+          <t>317000</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,12 +488,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>08/07/2024 11:49:45</t>
+          <t>22/07/2024 15:43:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>08/07/2024 11:50:01</t>
+          <t>22/07/2024 18:31:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -505,16 +505,16 @@
         <v>1500</v>
       </c>
       <c r="G2" t="n">
-        <v>16</v>
+        <v>10080</v>
       </c>
       <c r="H2" t="n">
-        <v>1500</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>310002</t>
+          <t>317001</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -524,12 +524,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>08/07/2024 18:11:30</t>
+          <t>22/07/2024 19:14:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>09/07/2024 12:12:09</t>
+          <t>22/07/2024 19:18:00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -541,16 +541,16 @@
         <v>1500</v>
       </c>
       <c r="G3" t="n">
-        <v>64839</v>
+        <v>240</v>
       </c>
       <c r="H3" t="n">
-        <v>14000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>310003</t>
+          <t>317002</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -560,12 +560,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>08/07/2024 18:11:38</t>
+          <t>22/07/2024 19:17:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>09/07/2024 12:13:47</t>
+          <t>22/07/2024 19:25:00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -577,190 +577,10 @@
         <v>1500</v>
       </c>
       <c r="G4" t="n">
-        <v>64929</v>
+        <v>480</v>
       </c>
       <c r="H4" t="n">
-        <v>14750</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>310004</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>CCC01</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>08/07/2024 18:11:43</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>09/07/2024 12:14:26</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Moto</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
         <v>1500</v>
-      </c>
-      <c r="G5" t="n">
-        <v>64963</v>
-      </c>
-      <c r="H5" t="n">
-        <v>14750</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>310005</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>DDD01</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>08/07/2024 18:11:54</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>09/07/2024 15:13:41</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Moto</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>1500</v>
-      </c>
-      <c r="G6" t="n">
-        <v>75707</v>
-      </c>
-      <c r="H6" t="n">
-        <v>14750</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>310006</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>EEE01</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>08/07/2024 18:12:11</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>09/07/2024 15:14:11</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Moto</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>1500</v>
-      </c>
-      <c r="G7" t="n">
-        <v>75720</v>
-      </c>
-      <c r="H7" t="n">
-        <v>14750</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>310007</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>FFF01</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>08/07/2024 18:17:30</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>09/07/2024 15:15:15</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Moto</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>1500</v>
-      </c>
-      <c r="G8" t="n">
-        <v>75465</v>
-      </c>
-      <c r="H8" t="n">
-        <v>15500</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>310008</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>GGG01</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>08/07/2024 18:18:07</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>09/07/2024 15:15:26</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Moto</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="G9" t="n">
-        <v>75439</v>
-      </c>
-      <c r="H9" t="n">
-        <v>15500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregó el prefijo de factura a configuración
</commit_message>
<xml_diff>
--- a/upload/xls/register.xlsx
+++ b/upload/xls/register.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Recibo</t>
+          <t>Factura</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>317000</t>
+          <t>FE-0317000</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -514,7 +514,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>317001</t>
+          <t>FE-0317001</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -550,7 +550,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>317002</t>
+          <t>FE-0317002</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -565,7 +565,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>22/07/2024 19:25:00</t>
+          <t>27/07/2024 08:10:00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -574,12 +574,84 @@
         </is>
       </c>
       <c r="F4" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G4" t="n">
+        <v>391980</v>
+      </c>
+      <c r="H4" t="n">
+        <v>64500</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>FE-0317003</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CCC001</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>22/07/2024 21:17:00</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>27/07/2024 08:17:00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Carro</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>16000</v>
+      </c>
+      <c r="G5" t="n">
+        <v>385200</v>
+      </c>
+      <c r="H5" t="n">
+        <v>144000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FE-0317004</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>27/07/2024 07:21:00</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>27/07/2024 08:18:00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
         <v>1500</v>
       </c>
-      <c r="G4" t="n">
-        <v>480</v>
-      </c>
-      <c r="H4" t="n">
+      <c r="G6" t="n">
+        <v>3420</v>
+      </c>
+      <c r="H6" t="n">
         <v>1500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agregó el prefijo de la factura en exportar a excel y en los recibos se agregaron ceros a la izquierda del consecutivo
</commit_message>
<xml_diff>
--- a/upload/xls/register.xlsx
+++ b/upload/xls/register.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FE-0317000</t>
+          <t>FE-0317055</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,12 +488,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>22/07/2024 15:43:00</t>
+          <t>29/07/2024 15:57:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>22/07/2024 18:31:00</t>
+          <t>29/07/2024 15:58:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -505,31 +505,31 @@
         <v>1500</v>
       </c>
       <c r="G2" t="n">
-        <v>10080</v>
+        <v>60</v>
       </c>
       <c r="H2" t="n">
-        <v>4500</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FE-0317001</t>
+          <t>FE-0317056</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AAA01</t>
+          <t>BBB01</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>22/07/2024 19:14:00</t>
+          <t>29/07/2024 16:38:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>22/07/2024 19:18:00</t>
+          <t>29/07/2024 16:55:00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -541,7 +541,7 @@
         <v>1500</v>
       </c>
       <c r="G3" t="n">
-        <v>240</v>
+        <v>1020</v>
       </c>
       <c r="H3" t="n">
         <v>1500</v>
@@ -550,22 +550,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FE-0317002</t>
+          <t>FE-0317057</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BBB01</t>
+          <t>CCC01</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>22/07/2024 19:17:00</t>
+          <t>29/07/2024 17:10:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>27/07/2024 08:10:00</t>
+          <t>29/07/2024 18:27:00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -574,85 +574,13 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>7000</v>
+        <v>1500</v>
       </c>
       <c r="G4" t="n">
-        <v>391980</v>
+        <v>4620</v>
       </c>
       <c r="H4" t="n">
-        <v>64500</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>FE-0317003</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>CCC001</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>22/07/2024 21:17:00</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>27/07/2024 08:17:00</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Carro</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>16000</v>
-      </c>
-      <c r="G5" t="n">
-        <v>385200</v>
-      </c>
-      <c r="H5" t="n">
-        <v>144000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>FE-0317004</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>AAA01</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>27/07/2024 07:21:00</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>27/07/2024 08:18:00</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Moto</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>1500</v>
-      </c>
-      <c r="G6" t="n">
-        <v>3420</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1500</v>
+        <v>3000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregó el textbox clave_tecnica, el switch billing_switch, el dropdown environment en configuración
</commit_message>
<xml_diff>
--- a/upload/xls/register.xlsx
+++ b/upload/xls/register.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -583,6 +583,42 @@
         <v>3000</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>FE-0317058</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>30/07/2024 11:17:00</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>30/07/2024 11:17:00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1500</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agregó la progressbar al exportar datos a excel en registro
</commit_message>
<xml_diff>
--- a/upload/xls/register.xlsx
+++ b/upload/xls/register.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FE-0317055</t>
+          <t>FE-0317000</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,12 +488,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>29/07/2024 15:57:00</t>
+          <t>07/08/2024 11:42:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>29/07/2024 15:58:00</t>
+          <t>07/08/2024 13:05:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -505,16 +505,16 @@
         <v>1500</v>
       </c>
       <c r="G2" t="n">
-        <v>60</v>
+        <v>4980</v>
       </c>
       <c r="H2" t="n">
-        <v>1500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FE-0317056</t>
+          <t>FE-0317001</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -524,12 +524,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>29/07/2024 16:38:00</t>
+          <t>07/08/2024 12:47:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>29/07/2024 16:55:00</t>
+          <t>07/08/2024 13:05:00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -541,81 +541,9 @@
         <v>1500</v>
       </c>
       <c r="G3" t="n">
-        <v>1020</v>
+        <v>1080</v>
       </c>
       <c r="H3" t="n">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>FE-0317057</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>CCC01</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>29/07/2024 17:10:00</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>29/07/2024 18:27:00</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Moto</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>1500</v>
-      </c>
-      <c r="G4" t="n">
-        <v>4620</v>
-      </c>
-      <c r="H4" t="n">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>FE-0317058</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>AAA01</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>30/07/2024 11:17:00</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>30/07/2024 11:17:00</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Moto</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
         <v>1500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se organizaron los cálculos, recibos y facturas, se agregó el botón de facturación
</commit_message>
<xml_diff>
--- a/upload/xls/register.xlsx
+++ b/upload/xls/register.xlsx
@@ -488,12 +488,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>07/08/2024 11:42:00</t>
+          <t>08/08/2024 15:23:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>07/08/2024 13:05:00</t>
+          <t>08/08/2024 15:23:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -505,10 +505,10 @@
         <v>1500</v>
       </c>
       <c r="G2" t="n">
-        <v>4980</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>3000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="3">
@@ -524,12 +524,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>07/08/2024 12:47:00</t>
+          <t>08/08/2024 17:40:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>07/08/2024 13:05:00</t>
+          <t>08/08/2024 17:40:00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -541,7 +541,7 @@
         <v>1500</v>
       </c>
       <c r="G3" t="n">
-        <v>1080</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
         <v>1500</v>

</xml_diff>

<commit_message>
Se modificó el número de recibos a imprimir por página en cuadre de caja
</commit_message>
<xml_diff>
--- a/upload/xls/register.xlsx
+++ b/upload/xls/register.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Factura</t>
+          <t>Recibo</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FE-0317000</t>
+          <t>317000</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -514,7 +514,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FE-0317001</t>
+          <t>317001</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -545,6 +545,1878 @@
       </c>
       <c r="H3" t="n">
         <v>1500</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>317002</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>09/08/2024 09:23:00</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>09/08/2024 09:46:00</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1380</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>317003</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BBB01</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>09/08/2024 09:45:00</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>09/08/2024 17:32:00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G5" t="n">
+        <v>28020</v>
+      </c>
+      <c r="H5" t="n">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>317004</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CCC01</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>11/08/2024 02:05:00</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>12/08/2024 14:26:00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G6" t="n">
+        <v>130860</v>
+      </c>
+      <c r="H6" t="n">
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>317005</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>DDD01</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>14/08/2024 09:00:00</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>16/08/2024 09:20:00</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G7" t="n">
+        <v>174000</v>
+      </c>
+      <c r="H7" t="n">
+        <v>29500</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>317006</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>EEE01</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>14/08/2024 19:30:00</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>15/08/2024 21:53:00</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>94980</v>
+      </c>
+      <c r="H8" t="n">
+        <v>18500</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>317007</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:19:00</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:20:00</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G9" t="n">
+        <v>60</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>317008</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:23:00</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:23:00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>317009</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:26:00</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:26:00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>317010</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:31:00</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:31:00</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>317011</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:32:00</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:32:00</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>317012</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:34:00</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:34:00</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>317013</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:36:00</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:36:00</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>317014</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:37:00</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:37:00</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>317015</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:40:00</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:40:00</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>317016</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:42:00</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:43:00</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G18" t="n">
+        <v>60</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>317017</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:47:00</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:47:00</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>317018</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:51:00</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:51:00</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>317019</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:55:00</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:55:00</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>317020</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:56:00</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:56:00</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>317021</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:58:00</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>16/08/2024 10:58:00</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>317022</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:00:00</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:00:00</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>317023</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:13:00</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:13:00</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>317024</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:14:00</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:15:00</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G26" t="n">
+        <v>60</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>317025</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:21:00</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:21:00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>317026</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:30:00</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:31:00</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G28" t="n">
+        <v>60</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>317027</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:32:00</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:32:00</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>317028</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:39:00</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:39:00</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>317029</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:41:00</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:41:00</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>317030</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:42:00</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:42:00</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>317031</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:43:00</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>16/08/2024 11:43:00</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>317032</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:16:00</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:16:00</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>317033</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:20:00</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:20:00</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>317034</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:20:00</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:20:00</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>317035</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:27:00</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:27:00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>317036</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:27:00</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:28:00</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G38" t="n">
+        <v>60</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>317037</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:33:00</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:34:00</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G39" t="n">
+        <v>60</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>317038</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:35:00</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:36:00</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G40" t="n">
+        <v>60</v>
+      </c>
+      <c r="H40" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>317039</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:36:00</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:37:00</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G41" t="n">
+        <v>60</v>
+      </c>
+      <c r="H41" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>317040</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:44:00</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:44:00</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>317041</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:45:00</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:45:00</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>317042</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:46:00</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:46:00</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>317043</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:50:00</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:51:00</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G45" t="n">
+        <v>60</v>
+      </c>
+      <c r="H45" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>317044</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:54:00</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>16/08/2024 12:54:00</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>317045</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>16/08/2024 13:10:00</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>16/08/2024 13:10:00</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>317046</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>16/08/2024 13:11:00</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>16/08/2024 13:11:00</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>317047</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>16/08/2024 13:19:00</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>16/08/2024 13:19:00</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>317048</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>16/08/2024 13:22:00</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>16/08/2024 13:23:00</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G50" t="n">
+        <v>60</v>
+      </c>
+      <c r="H50" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>317049</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>16/08/2024 13:25:00</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>16/08/2024 13:25:00</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>317050</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>16/08/2024 13:30:00</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>16/08/2024 13:30:00</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>317051</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>16/08/2024 15:09:00</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>16/08/2024 15:10:00</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G53" t="n">
+        <v>60</v>
+      </c>
+      <c r="H53" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>317052</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>16/08/2024 15:14:00</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>16/08/2024 15:19:00</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G54" t="n">
+        <v>300</v>
+      </c>
+      <c r="H54" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>317053</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>AAA01</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>16/08/2024 15:19:00</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>16/08/2024 16:51:00</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G55" t="n">
+        <v>5520</v>
+      </c>
+      <c r="H55" t="n">
+        <v>3000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>